<commit_message>
REPORTGEN-1053: update compliance reports
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4356419B-9F13-479D-B68C-5B4A923EEB35}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF0D59E-7B02-4048-89DB-94F81BD12518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Snapshot date:</t>
   </si>
   <si>
-    <t>Technical Debt:</t>
-  </si>
-  <si>
     <t>Generated on:</t>
   </si>
   <si>
@@ -72,9 +69,6 @@
     <t>RepGen:TEXT;LAST_SNAPSHOT_DATE</t>
   </si>
   <si>
-    <t>RepGen:TEXT;METRIC_TECHNICAL_DEBT</t>
-  </si>
-  <si>
     <t>Application characteristics</t>
   </si>
   <si>
@@ -169,6 +163,12 @@
   </si>
   <si>
     <t>RepGen:TABLE;LIST_RULES_VIOLATIONS_BOOKMARKS_TABLE;METRICS=MISRA-CPP-2008,COUNT=-1,HEADER=NO</t>
+  </si>
+  <si>
+    <t>ISO Technical Debt:</t>
+  </si>
+  <si>
+    <t>RepGen:TEXT;OMG_TECHNICAL_DEBT</t>
   </si>
 </sst>
 </file>
@@ -493,7 +493,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>432089</xdr:colOff>
+      <xdr:colOff>258907</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>245918</xdr:rowOff>
     </xdr:to>
@@ -829,38 +829,38 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="16.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C2" s="6"/>
       <c r="D2" s="2"/>
@@ -868,96 +868,96 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D3" s="11"/>
       <c r="E3" s="12"/>
       <c r="F3" s="9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G3" s="15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D4" s="4"/>
       <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
-        <v>2</v>
+        <v>40</v>
       </c>
       <c r="G4" s="10" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B6" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" s="18" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+      <c r="D6" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="18" t="s">
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C7" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D7" s="23"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="D8" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="18" t="s">
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C9" t="s">
         <v>14</v>
-      </c>
-      <c r="D8" s="18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
-        <v>16</v>
       </c>
       <c r="D9" s="23"/>
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B12" s="19" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="2:15" ht="22.8" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
       <c r="B13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="E13" s="24" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="E13" s="24" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -981,43 +981,43 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.21875" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1040,47 +1040,47 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1097,43 +1097,43 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.21875" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.21875" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="89.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1156,47 +1156,47 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -1213,43 +1213,43 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.21875" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>20</v>
+      </c>
+      <c r="F1" s="20" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C1" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>20</v>
-      </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="G1" s="20" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1272,47 +1272,47 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.77734375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.21875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>25</v>
       </c>
-      <c r="B1" s="20" t="s">
+      <c r="D1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="E1" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="D1" s="20" t="s">
+      <c r="F1" s="20" t="s">
         <v>28</v>
       </c>
-      <c r="E1" s="20" t="s">
+      <c r="G1" s="20" t="s">
         <v>29</v>
       </c>
-      <c r="F1" s="20" t="s">
+      <c r="H1" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="G1" s="20" t="s">
-        <v>31</v>
-      </c>
-      <c r="H1" s="20" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1102: part 1, added and removed counts missing when no previous snapshot selected
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5BF0D59E-7B02-4048-89DB-94F81BD12518}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEE854E-5BD7-452A-9164-1AE1421A4C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -144,9 +144,6 @@
     <t>Findings summary for CAST under C-CPP Standards</t>
   </si>
   <si>
-    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=C-CPP,MORE=true,HEADER=NO</t>
-  </si>
-  <si>
     <t>RepGen:TABLE;QUALITY_TAGS_RULES_EVOLUTION;STD=AUTOSAR-CPP-2014,DESC=true,HEADER=NO</t>
   </si>
   <si>
@@ -169,6 +166,9 @@
   </si>
   <si>
     <t>RepGen:TEXT;OMG_TECHNICAL_DEBT</t>
+  </si>
+  <si>
+    <t>RepGen:TABLE;QUALITY_STANDARDS_EVOLUTION;STD=C-CPP,MORE=true,HEADER=NO,EVOLUTION=true</t>
   </si>
 </sst>
 </file>
@@ -829,26 +829,26 @@
   <dimension ref="B1:O14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.5546875" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
-    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5703125" customWidth="1"/>
-    <col min="12" max="12" width="14.28515625" customWidth="1"/>
-    <col min="13" max="13" width="36.7109375" customWidth="1"/>
-    <col min="14" max="14" width="12.85546875" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" customWidth="1"/>
+    <col min="5" max="5" width="11.88671875" customWidth="1"/>
+    <col min="6" max="6" width="18.6640625" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
+    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5546875" customWidth="1"/>
+    <col min="12" max="12" width="14.33203125" customWidth="1"/>
+    <col min="13" max="13" width="36.6640625" customWidth="1"/>
+    <col min="14" max="14" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
@@ -858,7 +858,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
       <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
@@ -868,7 +868,7 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="21" t="s">
         <v>0</v>
       </c>
@@ -884,7 +884,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="22" t="s">
         <v>1</v>
       </c>
@@ -894,16 +894,16 @@
       <c r="D4" s="4"/>
       <c r="E4" s="13"/>
       <c r="F4" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="G4" s="10" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B6" s="18" t="s">
         <v>8</v>
       </c>
@@ -914,13 +914,13 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C7" t="s">
         <v>11</v>
       </c>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C8" s="18" t="s">
         <v>12</v>
       </c>
@@ -928,7 +928,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
       <c r="C9" t="s">
         <v>14</v>
       </c>
@@ -936,12 +936,12 @@
       <c r="N9" s="17"/>
       <c r="O9" s="16"/>
     </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B12" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:15" ht="22.8" x14ac:dyDescent="0.3">
       <c r="B13" s="19" t="s">
         <v>15</v>
       </c>
@@ -955,9 +955,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
-        <v>33</v>
+        <v>41</v>
       </c>
       <c r="C14" s="23"/>
       <c r="D14" s="23"/>
@@ -981,18 +981,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="88.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="1" max="1" width="88.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1015,9 +1015,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1040,19 +1040,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1078,9 +1078,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1097,18 +1097,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="89.28515625" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="1" max="1" width="89.33203125" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1131,9 +1131,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1156,19 +1156,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1194,9 +1194,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -1213,18 +1213,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="24.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" customWidth="1"/>
-    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.85546875" customWidth="1"/>
-    <col min="6" max="6" width="42.28515625" customWidth="1"/>
-    <col min="7" max="7" width="44.7109375" customWidth="1"/>
+    <col min="2" max="2" width="24.5546875" customWidth="1"/>
+    <col min="3" max="3" width="27.6640625" customWidth="1"/>
+    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.88671875" customWidth="1"/>
+    <col min="6" max="6" width="42.33203125" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1247,9 +1247,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="25" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="26"/>
       <c r="C2" s="26"/>
@@ -1272,19 +1272,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.28515625" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.85546875" customWidth="1"/>
-    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.88671875" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1310,9 +1310,9 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
REPORTGEN-1180: Update CAST Logos PJG
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJG\cast-repos\report-gen\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEE854E-5BD7-452A-9164-1AE1421A4C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5024559-EBFD-46AF-87D2-AB466FE42F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">Summary!#REF!</definedName>
-    <definedName name="Application_Size" comment="TEXT;APPLICATION_SIZE_TYPE" localSheetId="0">Summary!$G$3</definedName>
+    <definedName name="Application_Size" comment="TEXT;APPLICATION_SIZE_TYPE" localSheetId="0">Summary!$G$4</definedName>
     <definedName name="EmpVersion" comment="TEXT;EMP_VERSION" localSheetId="0">Summary!$E$1</definedName>
-    <definedName name="TABLE_1" comment="TEXT;APPLICATION_NAME" localSheetId="0">Summary!$D$3:$D$3</definedName>
-    <definedName name="TABLE_3" comment="TEXT;METRIC_TECHNICAL_DEBT" localSheetId="0">Summary!$G$4</definedName>
-    <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">Summary!$D$4:$D$4</definedName>
+    <definedName name="TABLE_1" comment="TEXT;APPLICATION_NAME" localSheetId="0">Summary!$D$4:$D$4</definedName>
+    <definedName name="TABLE_3" comment="TEXT;METRIC_TECHNICAL_DEBT" localSheetId="0">Summary!$G$5</definedName>
+    <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">Summary!$D$5:$D$5</definedName>
     <definedName name="TABLE_5" comment="TEXT;TODAY_DATE" localSheetId="0">Summary!$F$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -375,7 +375,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -399,16 +399,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,10 +418,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -449,6 +449,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -486,52 +498,50 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>692727</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1168976</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>55418</xdr:rowOff>
+      <xdr:rowOff>17318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>258907</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>245918</xdr:rowOff>
+      <xdr:colOff>959386</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82909</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E348FB7-C4BC-49A7-BE34-45B36734435F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="3870613" y="254577"/>
-          <a:ext cx="1601066" cy="190500"/>
+          <a:off x="9221931" y="216477"/>
+          <a:ext cx="1037319" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -826,29 +836,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O14"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
@@ -858,7 +868,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
@@ -868,100 +878,108 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="2:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="9" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+    <row r="5" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="7" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D7" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D9" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="16"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="D10" s="23"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+    <row r="14" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -981,18 +999,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>33</v>
       </c>
@@ -1040,19 +1058,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1078,7 +1096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1097,18 +1115,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="89.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>35</v>
       </c>
@@ -1156,19 +1174,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1194,7 +1212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1213,18 +1231,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>37</v>
       </c>
@@ -1272,19 +1290,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>

</xml_diff>

<commit_message>
REPORTGEN-1178: update logos in all the report templates
</commit_message>
<xml_diff>
--- a/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
+++ b/CastReporting.Reporting.Core/Templates/Application/Compliance reports/C-CPP Standards Full Detailed Report.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Dev\ReportGenerator\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PJG\cast-repos\report-gen\CAST-ReportGenerator\CastReporting.Reporting.Core\Templates\Application\Compliance reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CEE854E-5BD7-452A-9164-1AE1421A4C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5024559-EBFD-46AF-87D2-AB466FE42F5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="6" r:id="rId1"/>
@@ -23,11 +23,11 @@
   </sheets>
   <definedNames>
     <definedName name="AFP_LIST_TOTAL" comment="TABLE;AFP;TYPE=TOTAL" localSheetId="0">Summary!#REF!</definedName>
-    <definedName name="Application_Size" comment="TEXT;APPLICATION_SIZE_TYPE" localSheetId="0">Summary!$G$3</definedName>
+    <definedName name="Application_Size" comment="TEXT;APPLICATION_SIZE_TYPE" localSheetId="0">Summary!$G$4</definedName>
     <definedName name="EmpVersion" comment="TEXT;EMP_VERSION" localSheetId="0">Summary!$E$1</definedName>
-    <definedName name="TABLE_1" comment="TEXT;APPLICATION_NAME" localSheetId="0">Summary!$D$3:$D$3</definedName>
-    <definedName name="TABLE_3" comment="TEXT;METRIC_TECHNICAL_DEBT" localSheetId="0">Summary!$G$4</definedName>
-    <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">Summary!$D$4:$D$4</definedName>
+    <definedName name="TABLE_1" comment="TEXT;APPLICATION_NAME" localSheetId="0">Summary!$D$4:$D$4</definedName>
+    <definedName name="TABLE_3" comment="TEXT;METRIC_TECHNICAL_DEBT" localSheetId="0">Summary!$G$5</definedName>
+    <definedName name="TABLE_4" comment="TEXT;LAST_SNAPSHOT_DATE" localSheetId="0">Summary!$D$5:$D$5</definedName>
     <definedName name="TABLE_5" comment="TEXT;TODAY_DATE" localSheetId="0">Summary!$F$1:$G$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -375,7 +375,7 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -399,16 +399,16 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -418,10 +418,10 @@
     <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -449,6 +449,18 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -486,52 +498,50 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>692727</xdr:colOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>1168976</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>55418</xdr:rowOff>
+      <xdr:rowOff>17318</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>258907</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>245918</xdr:rowOff>
+      <xdr:colOff>959386</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>82909</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 7" descr="CAST_white_90">
+        <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E348FB7-C4BC-49A7-BE34-45B36734435F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+          <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:srcRect/>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
       </xdr:blipFill>
-      <xdr:spPr bwMode="auto">
+      <xdr:spPr>
         <a:xfrm>
-          <a:off x="3870613" y="254577"/>
-          <a:ext cx="1601066" cy="190500"/>
+          <a:off x="9221931" y="216477"/>
+          <a:ext cx="1037319" cy="360000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
         </a:prstGeom>
-        <a:noFill/>
-        <a:ln w="9525">
-          <a:noFill/>
-          <a:miter lim="800000"/>
-          <a:headEnd/>
-          <a:tailEnd/>
-        </a:ln>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -826,29 +836,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:O14"/>
+  <dimension ref="B1:O15"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.5546875" customWidth="1"/>
+    <col min="1" max="1" width="6.5703125" customWidth="1"/>
     <col min="2" max="2" width="66" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" customWidth="1"/>
-    <col min="5" max="5" width="11.88671875" customWidth="1"/>
-    <col min="6" max="6" width="18.6640625" customWidth="1"/>
-    <col min="7" max="7" width="19.44140625" customWidth="1"/>
-    <col min="8" max="8" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.5546875" customWidth="1"/>
-    <col min="12" max="12" width="14.33203125" customWidth="1"/>
-    <col min="13" max="13" width="36.6640625" customWidth="1"/>
-    <col min="14" max="14" width="12.88671875" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="8" max="8" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" customWidth="1"/>
+    <col min="13" max="13" width="36.7109375" customWidth="1"/>
+    <col min="14" max="14" width="12.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D1" s="3" t="s">
         <v>2</v>
       </c>
@@ -858,7 +868,7 @@
       <c r="F1" s="27"/>
       <c r="G1" s="27"/>
     </row>
-    <row r="2" spans="2:15" ht="23.4" x14ac:dyDescent="0.3">
+    <row r="2" spans="2:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
         <v>31</v>
       </c>
@@ -868,100 +878,108 @@
       <c r="F2" s="2"/>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="21" t="s">
+    <row r="3" spans="2:15" ht="15.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="28"/>
+      <c r="C3" s="29"/>
+      <c r="D3" s="30"/>
+      <c r="E3" s="30"/>
+      <c r="F3" s="30"/>
+      <c r="G3" s="31"/>
+    </row>
+    <row r="4" spans="2:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C4" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="9" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="15" t="s">
+      <c r="G4" s="15" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="22" t="s">
+    <row r="5" spans="2:15" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="22" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="7" t="s">
+      <c r="D5" s="4"/>
+      <c r="E5" s="13"/>
+      <c r="F5" s="7" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="10" t="s">
+      <c r="G5" s="10" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="5" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G5" s="14"/>
-    </row>
-    <row r="6" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B6" s="18" t="s">
+    <row r="6" spans="2:15" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B7" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="18" t="s">
+      <c r="C7" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D6" s="18" t="s">
+      <c r="D7" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+    <row r="8" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C8" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="23"/>
-    </row>
-    <row r="8" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C8" s="18" t="s">
+      <c r="D8" s="23"/>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C9" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="18" t="s">
+      <c r="D9" s="18" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="9" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+    <row r="10" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
         <v>14</v>
       </c>
-      <c r="D9" s="23"/>
-      <c r="N9" s="17"/>
-      <c r="O9" s="16"/>
-    </row>
-    <row r="12" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B12" s="19" t="s">
+      <c r="D10" s="23"/>
+      <c r="N10" s="17"/>
+      <c r="O10" s="16"/>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B13" s="19" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="2:15" ht="22.8" x14ac:dyDescent="0.3">
-      <c r="B13" s="19" t="s">
+    <row r="14" spans="2:15" ht="22.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="19" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C14" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="D14" s="24" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="E14" s="24" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="14" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B14" t="s">
+    <row r="15" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B15" t="s">
         <v>41</v>
       </c>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="23"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -981,18 +999,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="88.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1015,7 +1033,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>33</v>
       </c>
@@ -1040,19 +1058,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1078,7 +1096,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>34</v>
       </c>
@@ -1097,18 +1115,18 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="89.33203125" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="1" max="1" width="89.28515625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1131,7 +1149,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>35</v>
       </c>
@@ -1156,19 +1174,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1194,7 +1212,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>36</v>
       </c>
@@ -1213,18 +1231,18 @@
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="101" customWidth="1"/>
-    <col min="2" max="2" width="24.5546875" customWidth="1"/>
-    <col min="3" max="3" width="27.6640625" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="37.88671875" customWidth="1"/>
-    <col min="6" max="6" width="42.33203125" customWidth="1"/>
-    <col min="7" max="7" width="44.6640625" customWidth="1"/>
+    <col min="2" max="2" width="24.5703125" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" customWidth="1"/>
+    <col min="4" max="4" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="37.85546875" customWidth="1"/>
+    <col min="6" max="6" width="42.28515625" customWidth="1"/>
+    <col min="7" max="7" width="44.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>19</v>
       </c>
@@ -1247,7 +1265,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="25" t="s">
         <v>37</v>
       </c>
@@ -1272,19 +1290,19 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="94" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="51.33203125" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.88671875" customWidth="1"/>
-    <col min="7" max="7" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.28515625" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.85546875" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="20" t="s">
         <v>23</v>
       </c>
@@ -1310,7 +1328,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>

</xml_diff>